<commit_message>
Added class diagram and updated use cases
Added class diagram and updated use case.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Desktop\git\Portfolio-Manager\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\SE2 Project\Portfolio-Manager\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1FD289-ECC3-4F6B-814E-32A284EC6204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55016E-78CE-4E0D-9E34-3E5D730A6737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1335" yWindow="2040" windowWidth="20190" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Allow for the selling of crypto (server will handle this later)</t>
+  </si>
+  <si>
+    <t>Aayush</t>
   </si>
 </sst>
 </file>
@@ -1446,24 +1449,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="15.7265625" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +1491,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1519,9 +1522,9 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1544,8 +1547,10 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1567,8 +1572,10 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1590,8 +1597,10 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1622,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1636,7 +1645,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1659,7 +1668,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1684,7 +1693,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1707,7 +1716,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -1730,7 +1739,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1753,8 +1762,10 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1776,7 +1787,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1812,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>28</v>
@@ -1824,7 +1835,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>29</v>
@@ -1847,7 +1858,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>32</v>
@@ -1870,7 +1881,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>30</v>
@@ -1893,7 +1904,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>33</v>
@@ -1916,7 +1927,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>31</v>
@@ -1939,7 +1950,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1956,7 +1967,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1973,7 +1984,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1990,7 +2001,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2007,7 +2018,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2024,7 +2035,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
@@ -2095,13 +2106,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2115,205 +2126,205 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="1"/>
       <c r="C31" s="10"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="1"/>
       <c r="C32" s="10"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="1"/>
       <c r="C33" s="10"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="10"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated the documentation and added the UI wireframe for the user's landing page.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\SE2 Project\Portfolio-Manager\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Portfolio-Manager\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55016E-78CE-4E0D-9E34-3E5D730A6737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDFC340-C126-442D-96AF-F2CFA08C7E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="2040" windowWidth="20190" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -80,15 +80,6 @@
     <t>Allow for the verification of login information</t>
   </si>
   <si>
-    <t>Design the landing page (refer to wireframe)</t>
-  </si>
-  <si>
-    <t>Design the log in page (refer to wireframe)</t>
-  </si>
-  <si>
-    <t>Design the sign up page (refer to wireframe)</t>
-  </si>
-  <si>
     <t>Day 8</t>
   </si>
   <si>
@@ -141,6 +132,18 @@
   </si>
   <si>
     <t>Aayush</t>
+  </si>
+  <si>
+    <t>Designed the landing page for the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design the user landing page </t>
+  </si>
+  <si>
+    <t>Design the log in page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design the sign up page </t>
   </si>
 </sst>
 </file>
@@ -1449,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -1499,22 +1502,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1524,7 +1527,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1549,7 +1552,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -1574,7 +1577,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -1599,7 +1602,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -1673,7 +1676,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1694,9 +1697,11 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1717,9 +1722,11 @@
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1742,7 +1749,7 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1764,10 +1771,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -1792,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1815,7 +1822,7 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
         <v>1.5</v>
@@ -1838,7 +1845,7 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>1.5</v>
@@ -1861,7 +1868,7 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>1.5</v>
@@ -1884,7 +1891,7 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
         <v>1.5</v>
@@ -1907,7 +1914,7 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>1.5</v>
@@ -1930,7 +1937,7 @@
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -2100,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>7</v>
@@ -2117,7 +2124,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C30" s="10">
         <v>1</v>
@@ -2127,10 +2134,18 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11">
+        <v>45704</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -2330,7 +2345,7 @@
       </c>
       <c r="C64" s="3">
         <f>SUM(C30:C63)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64" s="9"/>
     </row>

</xml_diff>

<commit_message>
Updated the sprint 1 backlog
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Portfolio-Manager\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Desktop\git\Portfolio-Manager\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDFC340-C126-442D-96AF-F2CFA08C7E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B262464-2AF3-404B-98A3-DDC0FFAD431A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">Design the sign up page </t>
+  </si>
+  <si>
+    <t>Designed the sign up page</t>
   </si>
 </sst>
 </file>
@@ -1452,24 +1455,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1494,7 +1497,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1525,7 +1528,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -1550,7 +1553,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -1575,7 +1578,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -1600,7 +1603,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
@@ -1625,7 +1628,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1648,7 +1651,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1671,7 +1674,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1696,7 +1699,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1721,7 +1724,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
@@ -1746,7 +1749,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -1769,7 +1772,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
@@ -1794,7 +1797,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1819,7 +1822,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
@@ -1842,7 +1845,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>26</v>
@@ -1865,7 +1868,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
@@ -1888,7 +1891,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -1911,7 +1914,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>30</v>
@@ -1934,7 +1937,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -1957,7 +1960,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1974,7 +1977,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1991,7 +1994,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2008,7 +2011,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2025,7 +2028,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2042,7 +2045,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
@@ -2113,13 +2116,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2147,205 +2150,213 @@
         <v>45704</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="11">
+        <v>45705</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="1"/>
       <c r="C33" s="10"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="10"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="7"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="7"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="7"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="7"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="7"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="7"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="7"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="7"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="7"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="7"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="7"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="3">
         <f>SUM(C30:C63)</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D64" s="9"/>
     </row>

</xml_diff>

<commit_message>
Update Sprint 1 Backlog
Updated Sprint 1 Backlog with completed task, implementing the Account class, and the next planned task, integrating the login process with the view.
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Desktop\git\Portfolio-Manager\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blunt\Desktop\Portfolio-Manager\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B262464-2AF3-404B-98A3-DDC0FFAD431A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0B2A60-8467-435E-B0B5-52A13A69C3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22290" yWindow="2910" windowWidth="21555" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Designed the sign up page</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Implemented Account class</t>
   </si>
 </sst>
 </file>
@@ -1456,23 +1462,23 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="44.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="15.7265625" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1503,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1528,7 +1534,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1559,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -1578,7 +1584,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -1603,7 +1609,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
@@ -1628,7 +1634,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1651,7 +1657,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1674,7 +1680,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1699,7 +1705,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1724,7 +1730,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
@@ -1749,8 +1755,10 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1772,7 +1780,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
@@ -1797,7 +1805,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1822,8 +1830,10 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1845,7 +1855,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>26</v>
@@ -1868,7 +1878,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
@@ -1891,7 +1901,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -1914,7 +1924,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>30</v>
@@ -1937,7 +1947,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -1960,7 +1970,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1977,7 +1987,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1994,7 +2004,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2011,7 +2021,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2028,7 +2038,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2045,7 +2055,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2102,7 +2112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
@@ -2116,13 +2126,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2136,7 +2146,7 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2150,7 +2160,7 @@
         <v>45704</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
@@ -2164,199 +2174,207 @@
         <v>45705</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1</v>
+      </c>
+      <c r="D33" s="11">
+        <v>45703</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="1"/>
       <c r="C34" s="10"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="3">
         <f>SUM(C30:C63)</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="D64" s="9"/>
     </row>

</xml_diff>

<commit_message>
Updates the sprint 1 backlog
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Desktop\git\Portfolio-Manager\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project-physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1FD289-ECC3-4F6B-814E-32A284EC6204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D262E76-4C21-44C4-AAC4-5C7EE7A1A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="2385" windowWidth="20190" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -80,15 +80,6 @@
     <t>Allow for the verification of login information</t>
   </si>
   <si>
-    <t>Design the landing page (refer to wireframe)</t>
-  </si>
-  <si>
-    <t>Design the log in page (refer to wireframe)</t>
-  </si>
-  <si>
-    <t>Design the sign up page (refer to wireframe)</t>
-  </si>
-  <si>
     <t>Day 8</t>
   </si>
   <si>
@@ -138,6 +129,36 @@
   </si>
   <si>
     <t>Allow for the selling of crypto (server will handle this later)</t>
+  </si>
+  <si>
+    <t>Aayush</t>
+  </si>
+  <si>
+    <t>Designed the landing page for the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design the user landing page </t>
+  </si>
+  <si>
+    <t>Design the log in page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design the sign up page </t>
+  </si>
+  <si>
+    <t>Designed the sign up page</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Implemented Account class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented Crypto class </t>
+  </si>
+  <si>
+    <t>Implemented Crypto manager class</t>
   </si>
 </sst>
 </file>
@@ -369,7 +390,7 @@
                   <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1446,24 +1467,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="44.90625" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="15.7265625" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>2</v>
@@ -1488,7 +1509,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1496,22 +1517,22 @@
         <v>3</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -1519,9 +1540,9 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -1530,7 +1551,7 @@
         <v>1.5</v>
       </c>
       <c r="D3" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1544,8 +1565,10 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1553,7 +1576,7 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1567,8 +1590,10 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1590,8 +1615,10 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1613,7 +1640,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1636,7 +1663,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1659,12 +1686,12 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1684,10 +1711,12 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1707,10 +1736,12 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1730,10 +1761,12 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1753,10 +1786,12 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -1776,12 +1811,12 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1801,10 +1836,12 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
         <v>1.5</v>
@@ -1824,10 +1861,10 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>1.5</v>
@@ -1847,10 +1884,10 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>1.5</v>
@@ -1870,10 +1907,10 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
         <v>1.5</v>
@@ -1893,10 +1930,10 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>1.5</v>
@@ -1916,10 +1953,10 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -1939,7 +1976,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1956,7 +1993,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1973,7 +2010,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1990,7 +2027,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2007,7 +2044,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2024,7 +2061,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2034,7 +2071,7 @@
       </c>
       <c r="D26" s="3">
         <f>SUM(D3:D25)</f>
-        <v>26.5</v>
+        <v>23.5</v>
       </c>
       <c r="E26" s="3">
         <f>SUM(E3:E25)</f>
@@ -2081,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
@@ -2089,24 +2126,24 @@
         <v>1</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C30" s="10">
         <v>1</v>
@@ -2115,211 +2152,251 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11">
+        <v>45704</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="11">
+        <v>45705</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="10">
+        <v>1</v>
+      </c>
+      <c r="D33" s="11">
+        <v>45703</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="10">
+        <v>1</v>
+      </c>
+      <c r="D34" s="11">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="1"/>
       <c r="C36" s="10"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="3">
         <f>SUM(C30:C63)</f>
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="D64" s="9"/>
     </row>

</xml_diff>

<commit_message>
Integrated the data to be shown on the view
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 1 Backlog.xlsx
+++ b/Documentation/Sprint 1 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project-physics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Desktop\git\Portfolio-Manager\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D262E76-4C21-44C4-AAC4-5C7EE7A1A8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C29EB0-87B5-42F9-99BB-4345FA582A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2385" windowWidth="20190" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Task Manager / Dev</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Implemented Crypto manager class</t>
+  </si>
+  <si>
+    <t>Integrate the viewing of the crypto data to the view</t>
   </si>
 </sst>
 </file>
@@ -1467,24 +1470,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1512,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1540,7 +1543,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -1565,7 +1568,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1593,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>31</v>
       </c>
@@ -1615,7 +1618,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
@@ -1640,7 +1643,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -1663,7 +1666,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1686,7 +1689,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1711,7 +1714,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
@@ -1736,7 +1739,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
@@ -1761,7 +1764,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1786,9 +1789,9 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>22</v>
@@ -1811,7 +1814,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1839,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>37</v>
       </c>
@@ -1861,7 +1864,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>26</v>
@@ -1884,7 +1887,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>29</v>
@@ -1907,7 +1910,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
@@ -1930,7 +1933,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>30</v>
@@ -1953,7 +1956,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -1976,7 +1979,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1993,7 +1996,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2010,7 +2013,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2027,7 +2030,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2044,7 +2047,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2061,7 +2064,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
@@ -2132,13 +2135,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>45700</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>45704</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>45705</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>45703</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>31</v>
       </c>
@@ -2208,7 +2211,7 @@
         <v>45702</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
@@ -2222,181 +2225,189 @@
         <v>45702</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2</v>
+      </c>
+      <c r="D36" s="11">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
       <c r="B37" s="1"/>
       <c r="C37" s="10"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="1"/>
       <c r="C38" s="10"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
       <c r="B39" s="1"/>
       <c r="C39" s="10"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="7"/>
       <c r="B40" s="1"/>
       <c r="C40" s="10"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
       <c r="B41" s="1"/>
       <c r="C41" s="10"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="7"/>
       <c r="B42" s="1"/>
       <c r="C42" s="10"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="7"/>
       <c r="B43" s="1"/>
       <c r="C43" s="10"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="1"/>
       <c r="C44" s="10"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="7"/>
       <c r="B45" s="1"/>
       <c r="C45" s="10"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="7"/>
       <c r="B46" s="1"/>
       <c r="C46" s="10"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="7"/>
       <c r="B47" s="1"/>
       <c r="C47" s="10"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="7"/>
       <c r="B48" s="1"/>
       <c r="C48" s="10"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="7"/>
       <c r="B49" s="1"/>
       <c r="C49" s="10"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="7"/>
       <c r="B50" s="1"/>
       <c r="C50" s="10"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
       <c r="B51" s="1"/>
       <c r="C51" s="10"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
       <c r="B52" s="1"/>
       <c r="C52" s="10"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
       <c r="B53" s="1"/>
       <c r="C53" s="10"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="7"/>
       <c r="B54" s="1"/>
       <c r="C54" s="10"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="7"/>
       <c r="B55" s="1"/>
       <c r="C55" s="10"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="7"/>
       <c r="B56" s="1"/>
       <c r="C56" s="10"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="7"/>
       <c r="B57" s="1"/>
       <c r="C57" s="10"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="7"/>
       <c r="B58" s="1"/>
       <c r="C58" s="10"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="7"/>
       <c r="B59" s="1"/>
       <c r="C59" s="10"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="7"/>
       <c r="B60" s="1"/>
       <c r="C60" s="10"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="7"/>
       <c r="B61" s="1"/>
       <c r="C61" s="10"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="7"/>
       <c r="B62" s="1"/>
       <c r="C62" s="10"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="7"/>
       <c r="B63" s="1"/>
       <c r="C63" s="10"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="3">
         <f>SUM(C30:C63)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="D64" s="9"/>
     </row>

</xml_diff>